<commit_message>
all of my work after all this months
</commit_message>
<xml_diff>
--- a/Plots/Export graph.xlsx
+++ b/Plots/Export graph.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Random\ECON_P\Plots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Work\Export, Import\2020\10. Jan-Oct\Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB66696F-48C2-4C0A-8D5A-738B6B73DA34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51331DD6-243D-4807-9775-98988899672B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="15610" windowHeight="8610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Աճ</t>
   </si>
@@ -45,46 +50,70 @@
     <t>Կոնյակ, ռոմ, ջին, օղի, լիկյոր</t>
   </si>
   <si>
+    <t>Ալյումինե փայլաթիթեղներ&lt;0,2մմ</t>
+  </si>
+  <si>
+    <t>Մոլիբդենի հանքաքար, խտանյութ</t>
+  </si>
+  <si>
+    <t>Ադամանդե քար</t>
+  </si>
+  <si>
+    <t>Լոլիկ</t>
+  </si>
+  <si>
+    <t>Ոսկերչական իրեր</t>
+  </si>
+  <si>
     <t>Ոսկի անմշակ կամ կիսամշակ, փոշի</t>
   </si>
   <si>
-    <t xml:space="preserve">Հագուստ </t>
-  </si>
-  <si>
     <t>Երկաթամիահալվածք</t>
   </si>
   <si>
-    <t>Ալյումինե փայլաթիթեղներ&lt;0,2մմ</t>
-  </si>
-  <si>
-    <t>Թանկ. մետաղի թափոն եւ ջարդոն</t>
-  </si>
-  <si>
-    <t>Էլեկտրաէներգիա</t>
-  </si>
-  <si>
-    <t>Ադամանդե քար</t>
-  </si>
-  <si>
-    <t>Ոսկերչական իրեր</t>
+    <t>Ձուկ (թարմ)</t>
   </si>
   <si>
     <t>Ծիրան, բալ, դեղձ, կեռաս, հոն</t>
   </si>
   <si>
-    <t>Մոլիբդենի հանքաքար, խտանյութ</t>
-  </si>
-  <si>
     <t xml:space="preserve">Շոկոլադ </t>
   </si>
   <si>
+    <t>Ոչխարներ, այծեր (կենդանի)</t>
+  </si>
+  <si>
     <t>Հաշվիչ հեղուկի, գազի, էլեկտրաէներգիայի, մասեր</t>
   </si>
   <si>
+    <t>Ելակ, մոշ, մորի, թութ, հաղարջ, կիվի, նուռ</t>
+  </si>
+  <si>
+    <t>Պանիր, կաթնաշոռ</t>
+  </si>
+  <si>
     <t>Մրգային գինի</t>
   </si>
   <si>
-    <t>Պղինձ չզտված, պղնձե անոդ էլ. զտման համար</t>
+    <t>Խաղողի գինի, շամպայն</t>
+  </si>
+  <si>
+    <t>Խաղող, չամիչ</t>
+  </si>
+  <si>
+    <t>Վարունգ</t>
+  </si>
+  <si>
+    <t>Ոչխարի կամ այծի թարմ միս, պաղեցրած կամ սառեցրած</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Կոստյում, անդրավարտիք, պիջակ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Վերարկու, թիկնոց, անձրևանոց և նման հագուստ </t>
+  </si>
+  <si>
+    <t>Ժամացույցի թափք, մասեր</t>
   </si>
 </sst>
 </file>
@@ -94,7 +123,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +138,17 @@
       <name val="GHEA Grapalat"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="GHEA Grapalat"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="GHEA Grapalat"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +158,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -171,118 +211,45 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -558,214 +525,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5">
-        <v>625.66891185347072</v>
+      <c r="B2" s="6">
+        <v>522.1</v>
       </c>
       <c r="C2" s="6">
-        <v>100.35701636909209</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6">
+        <v>233.2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5">
-        <v>271.52934602976376</v>
-      </c>
-      <c r="C3" s="6">
-        <v>5.9212748481658082</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="6">
+        <v>191</v>
+      </c>
+      <c r="C4" s="6">
+        <v>-28.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5">
-        <v>245.70167717764596</v>
-      </c>
-      <c r="C4" s="6">
-        <v>50.9430705812361</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5">
-        <v>223.79517806223333</v>
+      <c r="B5" s="6">
+        <v>156</v>
       </c>
       <c r="C5" s="6">
-        <v>48.45182022873783</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>-36.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5">
-        <v>166.60724320949109</v>
+      <c r="B6" s="6">
+        <v>85.3</v>
       </c>
       <c r="C6" s="6">
-        <v>-58.395641943410681</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>72.599999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="6">
+        <v>78</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-3.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="6">
+        <v>77.7</v>
+      </c>
+      <c r="C8" s="7">
+        <v>-43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="6">
+        <v>35.9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6">
+        <v>29.2</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5">
-        <v>142.39842876469976</v>
-      </c>
-      <c r="C7" s="6">
-        <v>16.480479945883644</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="4" t="s">
+      <c r="B11" s="6">
+        <v>25.9</v>
+      </c>
+      <c r="C11" s="6">
+        <v>-18.100000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5">
-        <v>95.175273181392441</v>
-      </c>
-      <c r="C8" s="6">
-        <v>2.4415316960614888</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="4" t="s">
+      <c r="B12" s="6">
+        <v>25.7</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="6">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C13" s="6">
+        <v>-13.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="5">
-        <v>87.649279841814973</v>
-      </c>
-      <c r="C9" s="6">
-        <v>77.746179570587827</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5">
-        <v>62.927631803517535</v>
-      </c>
-      <c r="C10" s="6">
-        <v>-25.656143015836911</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5">
-        <v>53.54086210844001</v>
-      </c>
-      <c r="C11" s="6">
-        <v>-23.685055198336528</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5">
-        <v>41.226532209387038</v>
-      </c>
-      <c r="C12" s="6">
-        <v>7.0102310437314301</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5">
-        <v>23.873677385784163</v>
-      </c>
-      <c r="C13" s="6">
-        <v>-4.3664070880144692</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="6">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="C14" s="6">
+        <v>-15.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="6">
+        <v>13.3</v>
+      </c>
+      <c r="C15" s="6">
+        <v>-6.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
-        <v>17.861793526901867</v>
-      </c>
-      <c r="C14" s="6">
-        <v>10.220759965130402</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5">
-        <v>17.821642002289522</v>
-      </c>
-      <c r="C15" s="6">
-        <v>2.2162714977242111</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5">
-        <v>16.852966801956498</v>
+      <c r="B16" s="6">
+        <v>10.5</v>
       </c>
       <c r="C16" s="6">
-        <v>16.588874377682703</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5">
-        <v>14.307519200749297</v>
+      <c r="B17" s="6">
+        <v>10.4</v>
       </c>
       <c r="C17" s="6">
-        <v>6.0501993804631624</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
-      <c r="A18" s="7" t="s">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="6">
+        <v>10</v>
+      </c>
+      <c r="C18" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6">
+        <v>-7.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B20" s="6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="C20" s="6">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="6">
+        <v>8.6</v>
+      </c>
+      <c r="C21" s="6">
+        <v>-1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="6">
+        <v>7.8</v>
+      </c>
+      <c r="C22" s="6">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6">
+        <v>6.6</v>
+      </c>
+      <c r="C23" s="6">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="C24" s="6">
+        <v>-12.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C25" s="6">
+        <v>-2.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6">
         <v>0</v>
       </c>
-      <c r="C18" s="9">
-        <v>-58.457658543655143</v>
+      <c r="C26" s="6">
+        <v>-7.6</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C19" xr:uid="{BFD9BADA-7393-4973-A96C-4D2DFF7509DA}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C22">
+      <sortCondition descending="1" ref="C1:C19"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="B2:B30">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>